<commit_message>
Update wordpress_site_info.xlsx with latest site information
</commit_message>
<xml_diff>
--- a/wordpress_site_info.xlsx
+++ b/wordpress_site_info.xlsx
@@ -481,7 +481,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-08-01 01:28:43</t>
+          <t>2025-08-05 21:29:02</t>
         </is>
       </c>
     </row>
@@ -796,7 +796,7 @@
       </c>
       <c r="B8" s="5" t="inlineStr">
         <is>
-          <t>1.12.4</t>
+          <t>1.14</t>
         </is>
       </c>
       <c r="C8" s="5" t="inlineStr">
@@ -828,7 +828,7 @@
       </c>
       <c r="B9" s="5" t="inlineStr">
         <is>
-          <t>6.3.12</t>
+          <t>6.4.3</t>
         </is>
       </c>
       <c r="C9" s="5" t="inlineStr">
@@ -860,7 +860,7 @@
       </c>
       <c r="B10" s="5" t="inlineStr">
         <is>
-          <t>6.3.12</t>
+          <t>6.4.3</t>
         </is>
       </c>
       <c r="C10" s="5" t="inlineStr">
@@ -956,7 +956,7 @@
       </c>
       <c r="B13" s="5" t="inlineStr">
         <is>
-          <t>7.89</t>
+          <t>7.97</t>
         </is>
       </c>
       <c r="C13" s="5" t="inlineStr">
@@ -988,7 +988,7 @@
       </c>
       <c r="B14" s="5" t="inlineStr">
         <is>
-          <t>2.65</t>
+          <t>2.73</t>
         </is>
       </c>
       <c r="C14" s="5" t="inlineStr">
@@ -1052,7 +1052,7 @@
       </c>
       <c r="B16" s="5" t="inlineStr">
         <is>
-          <t>9.3.6</t>
+          <t>9.3.10</t>
         </is>
       </c>
       <c r="C16" s="5" t="inlineStr">
@@ -1084,7 +1084,7 @@
       </c>
       <c r="B17" s="5" t="inlineStr">
         <is>
-          <t>2.4.2</t>
+          <t>2.4.6</t>
         </is>
       </c>
       <c r="C17" s="5" t="inlineStr">
@@ -1116,7 +1116,7 @@
       </c>
       <c r="B18" s="5" t="inlineStr">
         <is>
-          <t>6.0.3</t>
+          <t>6.1</t>
         </is>
       </c>
       <c r="C18" s="5" t="inlineStr">
@@ -1176,7 +1176,7 @@
       </c>
       <c r="B20" s="5" t="inlineStr">
         <is>
-          <t>1.17.2</t>
+          <t>1.18.0</t>
         </is>
       </c>
       <c r="C20" s="5" t="inlineStr">
@@ -1208,7 +1208,7 @@
       </c>
       <c r="B21" s="5" t="inlineStr">
         <is>
-          <t>1.20.3</t>
+          <t>1.21.1</t>
         </is>
       </c>
       <c r="C21" s="5" t="inlineStr">
@@ -1336,7 +1336,7 @@
       </c>
       <c r="B25" s="5" t="inlineStr">
         <is>
-          <t>9.2.4</t>
+          <t>9.6.1</t>
         </is>
       </c>
       <c r="C25" s="5" t="inlineStr">
@@ -1368,7 +1368,7 @@
       </c>
       <c r="B26" s="5" t="inlineStr">
         <is>
-          <t>1.4.14</t>
+          <t>1.4.15</t>
         </is>
       </c>
       <c r="C26" s="5" t="inlineStr">
@@ -1400,7 +1400,7 @@
       </c>
       <c r="B27" s="5" t="inlineStr">
         <is>
-          <t>2.9.2</t>
+          <t>2.9.14</t>
         </is>
       </c>
       <c r="C27" s="5" t="inlineStr">
@@ -1496,7 +1496,7 @@
       </c>
       <c r="B30" s="5" t="inlineStr">
         <is>
-          <t>2.2.5</t>
+          <t>2.2.9</t>
         </is>
       </c>
       <c r="C30" s="5" t="inlineStr">
@@ -1556,7 +1556,7 @@
       </c>
       <c r="B32" s="5" t="inlineStr">
         <is>
-          <t>4.9.0</t>
+          <t>4.9.2</t>
         </is>
       </c>
       <c r="C32" s="5" t="inlineStr">
@@ -1620,7 +1620,7 @@
       </c>
       <c r="B34" s="5" t="inlineStr">
         <is>
-          <t>3.3.1</t>
+          <t>4.0.0</t>
         </is>
       </c>
       <c r="C34" s="5" t="inlineStr">
@@ -1652,7 +1652,7 @@
       </c>
       <c r="B35" s="5" t="inlineStr">
         <is>
-          <t>9.2.0</t>
+          <t>9.4.2</t>
         </is>
       </c>
       <c r="C35" s="5" t="inlineStr">
@@ -1684,7 +1684,7 @@
       </c>
       <c r="B36" s="5" t="inlineStr">
         <is>
-          <t>9.2.0</t>
+          <t>9.4.1</t>
         </is>
       </c>
       <c r="C36" s="5" t="inlineStr">
@@ -1716,7 +1716,7 @@
       </c>
       <c r="B37" s="5" t="inlineStr">
         <is>
-          <t>5.5.1</t>
+          <t>5.5.2</t>
         </is>
       </c>
       <c r="C37" s="5" t="inlineStr">
@@ -1876,7 +1876,7 @@
       </c>
       <c r="B42" s="5" t="inlineStr">
         <is>
-          <t>3.0.3</t>
+          <t>3.1.3</t>
         </is>
       </c>
       <c r="C42" s="5" t="inlineStr">
@@ -2004,7 +2004,7 @@
       </c>
       <c r="B46" s="5" t="inlineStr">
         <is>
-          <t>2.25.1.26</t>
+          <t>2.25.6.26</t>
         </is>
       </c>
       <c r="C46" s="5" t="inlineStr">
@@ -2036,7 +2036,7 @@
       </c>
       <c r="B47" s="5" t="inlineStr">
         <is>
-          <t>4.63.3</t>
+          <t>4.64.5</t>
         </is>
       </c>
       <c r="C47" s="5" t="inlineStr">
@@ -2068,7 +2068,7 @@
       </c>
       <c r="B48" s="5" t="inlineStr">
         <is>
-          <t>24.3</t>
+          <t>25.6</t>
         </is>
       </c>
       <c r="C48" s="5" t="inlineStr">
@@ -2100,7 +2100,7 @@
       </c>
       <c r="B49" s="5" t="inlineStr">
         <is>
-          <t>4.9.8</t>
+          <t>4.11.4</t>
         </is>
       </c>
       <c r="C49" s="5" t="inlineStr">
@@ -2132,7 +2132,7 @@
       </c>
       <c r="B50" s="5" t="inlineStr">
         <is>
-          <t>1.3.3</t>
+          <t>1.3.8</t>
         </is>
       </c>
       <c r="C50" s="5" t="inlineStr">
@@ -2196,7 +2196,7 @@
       </c>
       <c r="B52" s="5" t="inlineStr">
         <is>
-          <t>2.6.11</t>
+          <t>2.7.3</t>
         </is>
       </c>
       <c r="C52" s="5" t="inlineStr">
@@ -2228,7 +2228,7 @@
       </c>
       <c r="B53" s="5" t="inlineStr">
         <is>
-          <t>3.16.6</t>
+          <t>3.20.0</t>
         </is>
       </c>
       <c r="C53" s="5" t="inlineStr">

</xml_diff>

<commit_message>
Refactor code structure and remove redundant changes
</commit_message>
<xml_diff>
--- a/wordpress_site_info.xlsx
+++ b/wordpress_site_info.xlsx
@@ -481,7 +481,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-08-05 21:29:02</t>
+          <t>2025-08-05 22:09:16</t>
         </is>
       </c>
     </row>
@@ -505,7 +505,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>6.7.1</t>
+          <t>6.8.2</t>
         </is>
       </c>
     </row>

</xml_diff>